<commit_message>
commit thêm chức năng cập nhật khấu trừ....
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -163,13 +163,13 @@
         <v>20000.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>1500.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>2000.0</v>
+        <v>0.0</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>0.0</v>
@@ -189,7 +189,7 @@
         <v>20000.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>2000.0</v>
+        <v>1500.0</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>0.0</v>
@@ -215,13 +215,13 @@
         <v>20000.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>1500.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>1500.0</v>
+        <v>2000.0</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>0.0</v>
@@ -293,13 +293,13 @@
         <v>20000.0</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>0.0</v>
+        <v>2000.0</v>
       </c>
       <c r="E7" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>0.0</v>
+        <v>2000.0</v>
       </c>
       <c r="G7" t="n" s="0">
         <v>0.0</v>
@@ -325,7 +325,7 @@
         <v>0.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2000.0</v>
+        <v>1500.0</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>0.0</v>
@@ -345,13 +345,13 @@
         <v>20000.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>2000.0</v>
+        <v>1500.0</v>
       </c>
       <c r="E9" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>0.0</v>
+        <v>2000.0</v>
       </c>
       <c r="G9" t="n" s="0">
         <v>0.0</v>

</xml_diff>

<commit_message>
commit theo ý ní lên
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Bùi Thị Lan</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -160,22 +163,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>20000.0</v>
+        <v>2398.8462</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>1500.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>0.0</v>
+        <v>200.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>2000.0</v>
+        <v>3898.8462</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>3000.0</v>
+        <v>2198.8462</v>
       </c>
     </row>
     <row r="3">
@@ -186,22 +189,22 @@
         <v>9</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>20000.0</v>
+        <v>2398.8462</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>2000.0</v>
+        <v>1500.0</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>1500.0</v>
+        <v>4398.846</v>
       </c>
       <c r="G3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>3000.0</v>
+        <v>3898.8462</v>
       </c>
     </row>
     <row r="4">
@@ -212,22 +215,22 @@
         <v>10</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>20000.0</v>
+        <v>2398.8462</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>1500.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>1500.0</v>
+        <v>2398.8462</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>3000.0</v>
+        <v>2398.8462</v>
       </c>
     </row>
     <row r="5">
@@ -238,22 +241,22 @@
         <v>11</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>20000.0</v>
+        <v>2429.9998</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>0.0</v>
+        <v>1500.0</v>
       </c>
       <c r="E5" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>2000.0</v>
+        <v>3929.9998</v>
       </c>
       <c r="G5" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>3000.0</v>
+        <v>4430.0</v>
       </c>
     </row>
     <row r="6">
@@ -264,7 +267,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>20000.0</v>
+        <v>2429.9998</v>
       </c>
       <c r="D6" t="n" s="0">
         <v>2000.0</v>
@@ -273,13 +276,13 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>1500.0</v>
+        <v>2429.9998</v>
       </c>
       <c r="G6" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>3000.0</v>
+        <v>2429.9998</v>
       </c>
     </row>
     <row r="7">
@@ -290,22 +293,22 @@
         <v>13</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>20000.0</v>
+        <v>4159.0386</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>0.0</v>
+        <v>2000.0</v>
       </c>
       <c r="E7" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>0.0</v>
+        <v>5659.0386</v>
       </c>
       <c r="G7" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>3000.0</v>
+        <v>5659.0386</v>
       </c>
     </row>
     <row r="8">
@@ -316,7 +319,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>20000.0</v>
+        <v>4159.0386</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>2000.0</v>
@@ -325,13 +328,13 @@
         <v>0.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2000.0</v>
+        <v>6159.0386</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>3000.0</v>
+        <v>5659.0386</v>
       </c>
     </row>
     <row r="9">
@@ -342,22 +345,48 @@
         <v>15</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>20000.0</v>
+        <v>4159.0386</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>2000.0</v>
+        <v>1500.0</v>
       </c>
       <c r="E9" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>0.0</v>
+        <v>6159.0386</v>
       </c>
       <c r="G9" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>3000.0</v>
+        <v>6159.0386</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>2429.9998</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>4430.0</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>2429.9998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>